<commit_message>
se agrega ajustes a deseños de visita tecnica
</commit_message>
<xml_diff>
--- a/documentacion/desarrollo/diseño/visita tecnica/mockups diseños.xlsx
+++ b/documentacion/desarrollo/diseño/visita tecnica/mockups diseños.xlsx
@@ -9,15 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="opcion en menu visita tecnica" sheetId="4" r:id="rId1"/>
     <sheet name="creacion de visita técnica" sheetId="1" r:id="rId2"/>
-    <sheet name="Agregar observación" sheetId="2" r:id="rId3"/>
-    <sheet name="agreagar persona que interviene" sheetId="3" r:id="rId4"/>
+    <sheet name="tipo visita servicios publicos" sheetId="6" r:id="rId3"/>
+    <sheet name="Juridica vienes inmuebles" sheetId="7" r:id="rId4"/>
+    <sheet name="Agregar observación" sheetId="2" r:id="rId5"/>
+    <sheet name="agreagar persona que interviene" sheetId="3" r:id="rId6"/>
+    <sheet name="gestión de visitas tecnicas" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>calidad del inmueble</t>
   </si>
@@ -93,6 +97,27 @@
   </si>
   <si>
     <t>cargo</t>
+  </si>
+  <si>
+    <t>correo</t>
+  </si>
+  <si>
+    <t>suscriptor</t>
+  </si>
+  <si>
+    <t># medidor</t>
+  </si>
+  <si>
+    <t>Comodato</t>
+  </si>
+  <si>
+    <t>Arrendamiento</t>
+  </si>
+  <si>
+    <t>Administracíon</t>
+  </si>
+  <si>
+    <t>Restitución</t>
   </si>
 </sst>
 </file>
@@ -227,8 +252,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -250,16 +285,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -269,6 +294,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,33 +455,93 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>8283</xdr:rowOff>
+      <xdr:colOff>24848</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>16565</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>521805</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>16565</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>18636</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>26090</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagen 4"/>
+        <xdr:cNvPr id="6" name="Imagen 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1548848" y="6684065"/>
+          <a:ext cx="4582353" cy="1914525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1524000" y="6485283"/>
-          <a:ext cx="4580283" cy="1913282"/>
+          <a:off x="1524000" y="0"/>
+          <a:ext cx="4733925" cy="3619500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -462,10 +550,239 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>742949</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>182215</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1523999" y="3619500"/>
+          <a:ext cx="4714875" cy="1706215"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1543050" y="7258050"/>
+          <a:ext cx="4705350" cy="1914525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1533525" y="9525"/>
+          <a:ext cx="4733925" cy="3619500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>182215</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1543050" y="3619500"/>
+          <a:ext cx="4714875" cy="1706215"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1562099" y="7734300"/>
+          <a:ext cx="4772025" cy="1914525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -715,7 +1032,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -759,14 +1076,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>78028</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>58978</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -783,8 +1100,51 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1524000" y="1266826"/>
+          <a:off x="1524000" y="1819276"/>
           <a:ext cx="5343525" cy="525702"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2536</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1533525" y="0"/>
+          <a:ext cx="6089011" cy="3581400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1061,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,7 +1436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C20:X34"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="B25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G34" sqref="G34:I34"/>
     </sheetView>
   </sheetViews>
@@ -1134,48 +1494,50 @@
       </c>
     </row>
     <row r="29" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D29" s="1"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11" t="s">
+      <c r="D29" s="5"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="30" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="10"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="4"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="4"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="8"/>
     </row>
     <row r="31" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="G31" s="5"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="7"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="11"/>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="1"/>
+      <c r="D33" s="5"/>
       <c r="H33" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="9"/>
-      <c r="E34" s="10"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="10"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="4"/>
+      <c r="G34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="3"/>
+      <c r="I34" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1201,10 +1563,233 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C29:I37"/>
+  <sheetViews>
+    <sheetView topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:I34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="2.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="4"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="8"/>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G31" s="9"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="11"/>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C33" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="H33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="4"/>
+      <c r="G34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34" s="3"/>
+      <c r="I34" s="4"/>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C36" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" s="13"/>
+      <c r="G36" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" s="13"/>
+    </row>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C37" s="2"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="4"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="G30:I31"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:I37"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G34">
+      <formula1>$W$20:$W$27</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C30:E30">
+      <formula1>$X$20:$X$21</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C29:I40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="3.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="4"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="8"/>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G31" s="9"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="11"/>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C33" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="H33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="4"/>
+      <c r="G34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="3"/>
+      <c r="I34" s="4"/>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C36" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="G36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C37" s="2"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="4"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="4"/>
+    </row>
+    <row r="39" spans="3:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="G39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C40" s="2"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="4"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="G30:I31"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="G34:I34"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C30:E30">
+      <formula1>$X$20:$X$21</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G34">
+      <formula1>$W$20:$W$27</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C36:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39:E39"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,30 +1812,30 @@
       <c r="F37" s="13"/>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="9"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="8" t="s">
+      <c r="D39" s="3"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="10"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="4"/>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D40" s="9"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="8" t="s">
+      <c r="D40" s="3"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="10"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1266,24 +1851,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:I7"/>
+  <dimension ref="C4:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="B1" sqref="B1:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5" s="14" t="s">
@@ -1298,24 +1883,37 @@
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="10"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="C8:E8"/>
     <mergeCell ref="C7:I7"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="G6:I6"/>
@@ -1326,4 +1924,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
se agregam cambios en diseño
</commit_message>
<xml_diff>
--- a/documentacion/desarrollo/diseño/visita tecnica/mockups diseños.xlsx
+++ b/documentacion/desarrollo/diseño/visita tecnica/mockups diseños.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="opcion en menu visita tecnica" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>calidad del inmueble</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>Restitución</t>
+  </si>
+  <si>
+    <t>dfsasdfasdf</t>
+  </si>
+  <si>
+    <t>asdfasdfasdfasdf</t>
+  </si>
+  <si>
+    <t>documento</t>
   </si>
 </sst>
 </file>
@@ -1435,7 +1444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C20:X34"/>
   <sheetViews>
-    <sheetView topLeftCell="B34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="C31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G34" sqref="G34:I34"/>
     </sheetView>
   </sheetViews>
@@ -1504,7 +1513,7 @@
     </row>
     <row r="30" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C30" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="7"/>
@@ -1533,7 +1542,7 @@
       <c r="D34" s="6"/>
       <c r="E34" s="7"/>
       <c r="G34" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="7"/>
@@ -1564,8 +1573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C29:I37"/>
   <sheetViews>
-    <sheetView topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37:I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,10 +1639,14 @@
       <c r="H36" s="15"/>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C37" s="5"/>
+      <c r="C37" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="D37" s="6"/>
       <c r="E37" s="7"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="H37" s="6"/>
       <c r="I37" s="7"/>
     </row>
@@ -1758,17 +1771,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:E40"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="G30:I31"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="G34:I34"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:E40"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C30:E30">
@@ -1787,8 +1800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C36:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39:I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1855,7 +1868,7 @@
   <dimension ref="C4:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G9" sqref="G9:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1904,14 +1917,21 @@
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
+      <c r="G8" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
       <c r="D9" s="3"/>
       <c r="E9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="G9:I9"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="C7:I7"/>
     <mergeCell ref="C6:E6"/>
@@ -1929,7 +1949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:J13"/>
     </sheetView>
   </sheetViews>

</xml_diff>